<commit_message>
Fix annotations in example
</commit_message>
<xml_diff>
--- a/0.2.x/examples/reference-openbis-export/metadata.xlsx
+++ b/0.2.x/examples/reference-openbis-export/metadata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="18500" windowHeight="9280"/>
+    <workbookView activeTab="0" windowWidth="18580" windowHeight="9280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="90" count="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="92" count="92">
   <si>
     <t>Code</t>
   </si>
@@ -66,7 +66,10 @@
     <t>PUBLICATION</t>
   </si>
   <si>
-    <t>https://schema.org/creativeWork</t>
+    <t>https://schema.org/</t>
+  </si>
+  <si>
+    <t>https://schema.org/CreativeWork</t>
   </si>
   <si>
     <t>Mandatory</t>
@@ -129,6 +132,12 @@
   </si>
   <si>
     <t>Organization</t>
+  </si>
+  <si>
+    <t>schema.org</t>
+  </si>
+  <si>
+    <t>https://schema.org/version/28.1</t>
   </si>
   <si>
     <t>Type</t>
@@ -172,9 +181,9 @@
     <t>Creators</t>
   </si>
   <si>
-    <t>http://datacite.org/schema/kernel-4#creator
+    <t>http://datacite.org/schema/kernel-4#Creator
 https://schema.org/author
-https://schema.org/creator</t>
+https://schema.org/Creator</t>
   </si>
   <si>
     <t>Contributors</t>
@@ -190,10 +199,6 @@
   </si>
   <si>
     <t>Creator Identifier</t>
-  </si>
-  <si>
-    <t>http://datacite.org/schema/kernel-4#nameIdentifier
-https://schema.org/identifier</t>
   </si>
   <si>
     <t>Identifier Scheme</t>
@@ -409,13 +414,14 @@
   </sheetPr>
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView topLeftCell="A24" workbookViewId="0" tabSelected="1">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="1" style="1" width="74.1384014423077" customWidth="1"/>
+    <col min="2" max="16384" style="1" width="9.142307692307693"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15">
@@ -547,13 +553,11 @@
           <t>PUB</t>
         </is>
       </c>
-      <c r="G10" s="3" t="inlineStr">
-        <is>
-          <t>https://schema.org/</t>
-        </is>
+      <c r="G10" s="3" t="s">
+        <v>15</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I10" s="3" t="inlineStr">
         <is>
@@ -569,46 +573,46 @@
         <v>1</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q11" s="2" t="s">
         <v>11</v>
@@ -622,7 +626,7 @@
     </row>
     <row r="12" spans="1:22" ht="102">
       <c r="A12" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>4</v>
@@ -634,17 +638,17 @@
         <v>4</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
@@ -660,7 +664,7 @@
         <v>5</v>
       </c>
       <c r="Q12" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R12" s="4" t="inlineStr">
         <is>
@@ -669,7 +673,7 @@
         </is>
       </c>
       <c r="S12" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15">
@@ -688,17 +692,17 @@
         <v>4</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -713,20 +717,16 @@
       <c r="P13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Q13" s="3" t="inlineStr">
-        <is>
-          <t>schema.org</t>
-        </is>
+      <c r="Q13" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="R13" s="3" t="inlineStr">
         <is>
           <t>http://schema.org/Organization</t>
         </is>
       </c>
-      <c r="S13" s="3" t="inlineStr">
-        <is>
-          <t>https://schema.org/version/28.1</t>
-        </is>
+      <c r="S13" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15">
@@ -745,17 +745,17 @@
         <v>4</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -790,17 +790,17 @@
         <v>4</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -816,13 +816,13 @@
         <v>5</v>
       </c>
       <c r="Q15" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R15" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="S15" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15">
@@ -841,10 +841,10 @@
         <v>4</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G16" s="3" t="inlineStr">
         <is>
@@ -853,7 +853,7 @@
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -869,7 +869,7 @@
         <v>5</v>
       </c>
       <c r="Q16" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R16" s="4" t="inlineStr">
         <is>
@@ -878,7 +878,7 @@
         </is>
       </c>
       <c r="S16" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15">
@@ -897,13 +897,13 @@
         <v>4</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>2</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H17" s="3"/>
       <c r="I17" s="3" t="s">
@@ -923,7 +923,7 @@
         <v>5</v>
       </c>
       <c r="Q17" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R17" s="4" t="inlineStr">
         <is>
@@ -933,7 +933,7 @@
         </is>
       </c>
       <c r="S17" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15">
@@ -952,17 +952,17 @@
         <v>4</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
@@ -978,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="R18" s="3" t="inlineStr">
         <is>
@@ -986,7 +986,7 @@
         </is>
       </c>
       <c r="S18" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15">
@@ -1006,7 +1006,7 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="G19" s="3" t="inlineStr">
         <is>
@@ -1052,17 +1052,17 @@
         <v>4</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="J20" s="3"/>
       <c r="K20" s="3"/>
@@ -1078,7 +1078,7 @@
         <v>5</v>
       </c>
       <c r="Q20" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R20" s="4" t="inlineStr">
         <is>
@@ -1087,10 +1087,10 @@
         </is>
       </c>
       <c r="S20" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" ht="15">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" ht="135.75">
       <c r="A21" s="3" t="inlineStr">
         <is>
           <t>PUBLICATION.CREATOR</t>
@@ -1106,10 +1106,10 @@
         <v>4</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G21" s="3" t="inlineStr">
         <is>
@@ -1118,7 +1118,7 @@
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
@@ -1134,13 +1134,13 @@
         <v>5</v>
       </c>
       <c r="Q21" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="R21" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="S21" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15">
@@ -1159,17 +1159,17 @@
         <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
@@ -1185,16 +1185,16 @@
         <v>5</v>
       </c>
       <c r="Q22" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="S22" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="23" spans="1:22" ht="28.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" ht="113.25">
       <c r="A23" s="3" t="inlineStr">
         <is>
           <t>PUBLICATION.PUBLISHER</t>
@@ -1210,10 +1210,10 @@
         <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G23" s="3" t="inlineStr">
         <is>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="H23" s="3"/>
       <c r="I23" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
@@ -1238,16 +1238,16 @@
         <v>5</v>
       </c>
       <c r="Q23" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R23" s="4" t="inlineStr">
         <is>
           <t>http://datacite.org/schema/kernel-4#publisher
-https://schema.org/publisher</t>
+https://schema.org/Publisher</t>
         </is>
       </c>
       <c r="S23" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15">
@@ -1266,10 +1266,10 @@
         <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="G24" s="3" t="inlineStr">
         <is>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="H24" s="3"/>
       <c r="I24" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
@@ -1294,7 +1294,7 @@
         <v>5</v>
       </c>
       <c r="Q24" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R24" s="4" t="inlineStr">
         <is>
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="S24" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15"/>
@@ -1341,9 +1341,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:22" ht="15">
+    <row r="28" spans="1:22" ht="135.75">
       <c r="A28" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>5</v>
@@ -1359,13 +1359,13 @@
         </is>
       </c>
       <c r="G28" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H28" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="15">
@@ -1376,46 +1376,46 @@
         <v>1</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I29" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q29" s="2" t="s">
         <v>11</v>
@@ -1443,17 +1443,17 @@
         <v>4</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H30" s="3"/>
       <c r="I30" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
@@ -1469,13 +1469,16 @@
         <v>5</v>
       </c>
       <c r="Q30" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="R30" s="4" t="s">
-        <v>54</v>
+        <v>34</v>
+      </c>
+      <c r="R30" s="4" t="inlineStr">
+        <is>
+          <t>http://datacite.org/schema/kernel-4#nameIdentifier
+https://schema.org/identifier</t>
+        </is>
       </c>
       <c r="S30" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="15">
@@ -1494,17 +1497,17 @@
         <v>4</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H31" s="3"/>
       <c r="I31" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
@@ -1525,7 +1528,7 @@
     </row>
     <row r="32" spans="1:22" ht="113.25">
       <c r="A32" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>4</v>
@@ -1537,17 +1540,17 @@
         <v>4</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H32" s="3"/>
       <c r="I32" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
@@ -1563,7 +1566,7 @@
         <v>5</v>
       </c>
       <c r="Q32" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R32" s="4" t="inlineStr">
         <is>
@@ -1572,7 +1575,7 @@
         </is>
       </c>
       <c r="S32" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:22" ht="15">
@@ -1591,17 +1594,17 @@
         <v>4</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H33" s="3"/>
       <c r="I33" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
@@ -1617,7 +1620,7 @@
         <v>5</v>
       </c>
       <c r="Q33" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R33" s="4" t="inlineStr">
         <is>
@@ -1626,7 +1629,7 @@
         </is>
       </c>
       <c r="S33" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:22" ht="15">
@@ -1645,17 +1648,17 @@
         <v>4</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H34" s="3"/>
       <c r="I34" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
@@ -1671,7 +1674,7 @@
         <v>5</v>
       </c>
       <c r="Q34" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R34" s="4" t="inlineStr">
         <is>
@@ -1680,7 +1683,7 @@
         </is>
       </c>
       <c r="S34" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:22" ht="15">
@@ -1699,13 +1702,13 @@
         <v>4</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H35" s="3"/>
       <c r="I35" s="3" t="inlineStr">
@@ -1746,17 +1749,17 @@
         <v>4</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H36" s="3"/>
       <c r="I36" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
@@ -1791,17 +1794,17 @@
         <v>4</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H37" s="3"/>
       <c r="I37" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
@@ -1853,7 +1856,7 @@
     </row>
     <row r="41" spans="1:22" ht="15">
       <c r="A41" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>5</v>
@@ -1872,46 +1875,46 @@
         <v>1</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P42" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q42" s="2" t="s">
         <v>11</v>
@@ -1925,7 +1928,7 @@
     </row>
     <row r="43" spans="1:22" ht="15">
       <c r="A43" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>4</v>
@@ -1937,17 +1940,17 @@
         <v>4</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H43" s="3"/>
       <c r="I43" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
@@ -1982,13 +1985,13 @@
         <v>4</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H44" s="3"/>
       <c r="I44" s="3" t="inlineStr">
@@ -2029,10 +2032,10 @@
         <v>4</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G45" s="3" t="inlineStr">
         <is>
@@ -2101,7 +2104,7 @@
     </row>
     <row r="49" spans="1:22" ht="15">
       <c r="A49" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B49" s="3" t="s">
         <v>5</v>
@@ -2116,9 +2119,17 @@
           <t>PUBPUB</t>
         </is>
       </c>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H49" s="3" t="inlineStr">
+        <is>
+          <t>https://schema.org/Publisher</t>
+        </is>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="50" spans="1:22" ht="15">
       <c r="A50" s="2" t="s">
@@ -2128,46 +2139,46 @@
         <v>1</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="I50" s="2" t="s">
         <v>2</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="O50" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="P50" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q50" s="2" t="s">
         <v>11</v>
@@ -2195,17 +2206,17 @@
         <v>4</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="J51" s="3"/>
       <c r="K51" s="3"/>
@@ -2221,7 +2232,7 @@
         <v>5</v>
       </c>
       <c r="Q51" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="R51" s="4" t="inlineStr">
         <is>
@@ -2230,7 +2241,7 @@
         </is>
       </c>
       <c r="S51" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="52" spans="1:22" ht="15">
@@ -2249,17 +2260,17 @@
         <v>4</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H52" s="3"/>
       <c r="I52" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -2275,7 +2286,7 @@
         <v>5</v>
       </c>
       <c r="Q52" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="R52" s="3" t="inlineStr">
         <is>
@@ -2283,7 +2294,7 @@
         </is>
       </c>
       <c r="S52" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="53" spans="1:22" ht="15">
@@ -2302,17 +2313,17 @@
         <v>4</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H53" s="3"/>
       <c r="I53" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="J53" s="3"/>
       <c r="K53" s="3"/>
@@ -2328,7 +2339,7 @@
         <v>5</v>
       </c>
       <c r="Q53" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="R53" s="3" t="inlineStr">
         <is>
@@ -2336,12 +2347,12 @@
         </is>
       </c>
       <c r="S53" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="54" spans="1:22" ht="15">
       <c r="A54" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>4</v>
@@ -2353,17 +2364,17 @@
         <v>4</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="H54" s="3"/>
       <c r="I54" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
@@ -2400,7 +2411,7 @@
     </row>
     <row r="58" spans="1:22" ht="15">
       <c r="A58" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
@@ -2418,7 +2429,7 @@
     </row>
     <row r="61" spans="1:22" ht="15">
       <c r="A61" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>0</v>
@@ -2427,94 +2438,94 @@
         <v>2</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:22" ht="15">
       <c r="A62" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B62" s="3" t="inlineStr">
+        <is>
+          <t>PUBLIC_REPOSITORIES</t>
+        </is>
+      </c>
+      <c r="C62" s="3" t="inlineStr">
+        <is>
+          <t>Public Repositories</t>
+        </is>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="B62" s="3" t="inlineStr">
-        <is>
-          <t>PUBLIC_REPOSITORIES</t>
-        </is>
-      </c>
-      <c r="C62" s="3" t="inlineStr">
-        <is>
-          <t>Public Repositories</t>
-        </is>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="63" spans="1:22" ht="15"/>
     <row r="64" spans="1:22" ht="13.8">
       <c r="A64" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="65" spans="1:22" ht="13.8">
       <c r="A65" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="66" spans="1:22" ht="13.8">
       <c r="A66" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:22" ht="13.8">
       <c r="A67" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D67" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I67" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="L67" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M67" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="P67" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="Q67" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:22" ht="13.8">
@@ -2523,7 +2534,7 @@
         <v>5</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D68" s="2" t="inlineStr">
         <is>
@@ -2531,13 +2542,13 @@
         </is>
       </c>
       <c r="E68" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -2560,7 +2571,7 @@
         <v>5</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="D69" s="2" t="inlineStr">
         <is>
@@ -2568,13 +2579,13 @@
         </is>
       </c>
       <c r="E69" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G69" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -2601,21 +2612,21 @@
         <v>5</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" s="2" t="inlineStr">
+        <is>
+          <t>PUBCREA23</t>
+        </is>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="D70" s="2" t="inlineStr">
-        <is>
-          <t>PUBCREA23</t>
-        </is>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F70" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -2646,58 +2657,58 @@
     </row>
     <row r="72" spans="1:22" ht="13.8">
       <c r="A72" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="73" spans="1:22" ht="13.8">
       <c r="A73" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="74" spans="1:22" ht="13.8">
       <c r="A74" s="3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:22" ht="13.8">
       <c r="A75" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E75" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I75" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="J75" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K75" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="L75" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F75" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="J75" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="K75" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="L75" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="M75" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="76" spans="1:22" ht="13.8">
@@ -2706,7 +2717,7 @@
         <v>5</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D76" s="2" t="inlineStr">
         <is>
@@ -2714,13 +2725,13 @@
         </is>
       </c>
       <c r="E76" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2739,7 +2750,7 @@
         <v>5</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D77" s="2" t="inlineStr">
         <is>
@@ -2747,13 +2758,13 @@
         </is>
       </c>
       <c r="E77" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -2782,32 +2793,32 @@
     </row>
     <row r="81" spans="1:22" ht="13.8">
       <c r="A81" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="82" spans="1:22" ht="13.8">
       <c r="A82" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:22" ht="13.8">
       <c r="A83" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B83" s="2" t="inlineStr">
         <is>
@@ -2815,7 +2826,7 @@
         </is>
       </c>
       <c r="C83" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D83" s="2" t="inlineStr">
         <is>
@@ -2823,7 +2834,7 @@
         </is>
       </c>
       <c r="E83" s="2" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>6</v>
@@ -2831,7 +2842,7 @@
     </row>
     <row r="84" spans="1:22" ht="13.8">
       <c r="A84" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B84" s="2" t="inlineStr">
         <is>
@@ -2839,7 +2850,7 @@
         </is>
       </c>
       <c r="C84" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D84" s="2" t="inlineStr">
         <is>
@@ -2853,7 +2864,7 @@
     </row>
     <row r="85" spans="1:22" ht="13.8">
       <c r="A85" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B85" s="2" t="inlineStr">
         <is>
@@ -2861,7 +2872,7 @@
         </is>
       </c>
       <c r="C85" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="D85" s="2" t="inlineStr">
         <is>
@@ -2869,18 +2880,18 @@
         </is>
       </c>
       <c r="E85" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="F85" s="2"/>
     </row>
     <row r="87" spans="1:22" ht="13.8">
       <c r="A87" s="2" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
     </row>
     <row r="88" spans="1:22" ht="13.8">
       <c r="A88" s="2" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:22" ht="13.8">
@@ -2890,70 +2901,70 @@
     </row>
     <row r="90" spans="1:22" ht="13.8">
       <c r="A90" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>0</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G90" s="2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H90" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J90" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K90" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="N90" s="2" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="O90" s="2" t="s">
         <v>2</v>
       </c>
       <c r="P90" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="Q90" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="R90" s="2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="S90" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="T90" s="2" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="U90" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="V90" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="91" spans="1:22" ht="13.8">
@@ -2972,13 +2983,13 @@
         </is>
       </c>
       <c r="E91" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G91" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
@@ -2989,7 +3000,7 @@
       </c>
       <c r="K91" s="2"/>
       <c r="L91" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M91" s="2" t="inlineStr">
         <is>
@@ -3005,14 +3016,14 @@
       <c r="P91" s="2"/>
       <c r="Q91" s="2"/>
       <c r="R91" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="S91" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="T91" s="2"/>
       <c r="U91" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V91" s="2" t="inlineStr">
         <is>
@@ -3036,13 +3047,13 @@
         </is>
       </c>
       <c r="E92" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G92" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
@@ -3053,7 +3064,7 @@
       </c>
       <c r="K92" s="2"/>
       <c r="L92" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M92" s="2" t="inlineStr">
         <is>
@@ -3069,14 +3080,14 @@
       <c r="P92" s="2"/>
       <c r="Q92" s="2"/>
       <c r="R92" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="S92" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="T92" s="2"/>
       <c r="U92" s="2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="V92" s="2" t="inlineStr">
         <is>
@@ -3100,13 +3111,13 @@
         </is>
       </c>
       <c r="E93" s="2" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G93" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
@@ -3117,7 +3128,7 @@
       </c>
       <c r="K93" s="2"/>
       <c r="L93" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="M93" s="2" t="inlineStr">
         <is>
@@ -3133,14 +3144,14 @@
       <c r="P93" s="2"/>
       <c r="Q93" s="2"/>
       <c r="R93" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="S93" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="T93" s="2"/>
       <c r="U93" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="V93" s="2" t="inlineStr">
         <is>

</xml_diff>